<commit_message>
Change led from 1206 to 0805
</commit_message>
<xml_diff>
--- a/PCB_SOTB_LWC/SOTB_LWC_bom.xlsx
+++ b/PCB_SOTB_LWC/SOTB_LWC_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\backup\PCB_SOTB_LWC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE875BF-78AF-4F94-8A95-FCD5858FAA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E2C7C5-0648-4D78-8D4A-C761914BCE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,13 +72,6 @@
     </r>
   </si>
   <si>
-    <t>LEDCHIPLED_1206</t>
-  </si>
-  <si>
-    <t>C14641</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>C110255</t>
   </si>
   <si>
@@ -278,6 +271,12 @@
   </si>
   <si>
     <t>C1823</t>
+  </si>
+  <si>
+    <t>LEDCHIPLED_0805</t>
+  </si>
+  <si>
+    <t>C34499</t>
   </si>
 </sst>
 </file>
@@ -378,7 +377,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -408,6 +407,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,7 +796,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
@@ -824,16 +826,16 @@
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" s="6">
-        <v>1206</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
+        <v>805</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45.75" customHeight="1">
@@ -841,153 +843,153 @@
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C3" s="6">
         <v>1206</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="48" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C4" s="6">
         <v>1206</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="6">
         <v>805</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" s="6">
         <v>805</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" s="6">
         <v>805</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="6">
         <v>1206</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1206</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1206</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1206</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="6">
-        <v>1206</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1206</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="6">
-        <v>1206</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" s="6">
         <v>1206</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1206</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" s="6">
-        <v>1206</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -995,13 +997,13 @@
         <v>100</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" s="6">
         <v>1206</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1009,55 +1011,55 @@
         <v>4</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" s="6">
         <v>1206</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="6">
         <v>1206</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C17" s="6">
         <v>1206</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1206</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C18" s="6">
-        <v>1206</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1065,13 +1067,13 @@
         <v>330</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="6">
         <v>1206</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1079,69 +1081,69 @@
         <v>357</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" s="6">
         <v>1206</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="D22" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4">

</xml_diff>